<commit_message>
A lot of changes to make the code more transparent and hopefully more efficient.
</commit_message>
<xml_diff>
--- a/data/DRI EAR valuesV2.xlsx
+++ b/data/DRI EAR valuesV2.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="4" rupBuild="26004"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26207"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gcn/Documents/workspace/nutrientModeling/data/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="-28380" yWindow="-3660" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2480" yWindow="1040" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DRI -RDA&amp;AI" sheetId="2" r:id="rId1"/>
@@ -171,78 +176,12 @@
     <t>Lactation</t>
   </si>
   <si>
-    <t>ENERGYC</t>
-  </si>
-  <si>
-    <t>PROTC</t>
-  </si>
-  <si>
-    <t>FATC</t>
-  </si>
-  <si>
-    <t>CHOC</t>
-  </si>
-  <si>
-    <t>FIBC</t>
-  </si>
-  <si>
-    <t>CAC</t>
-  </si>
-  <si>
-    <t>PC</t>
-  </si>
-  <si>
-    <t>MGC</t>
-  </si>
-  <si>
-    <t>KC</t>
-  </si>
-  <si>
-    <t>NAC</t>
-  </si>
-  <si>
-    <t>FEC</t>
-  </si>
-  <si>
-    <t>ZNC</t>
-  </si>
-  <si>
     <t>CUC</t>
   </si>
   <si>
     <t>MNC</t>
   </si>
   <si>
-    <t>VITAC</t>
-  </si>
-  <si>
-    <t>VITDC</t>
-  </si>
-  <si>
-    <t>VITEC</t>
-  </si>
-  <si>
-    <t>VITCC</t>
-  </si>
-  <si>
-    <t>THIAC</t>
-  </si>
-  <si>
-    <t>RIBFC</t>
-  </si>
-  <si>
-    <t>NIAC</t>
-  </si>
-  <si>
-    <t>VITB6C</t>
-  </si>
-  <si>
-    <t>FOLC</t>
-  </si>
-  <si>
-    <t>VITB12C</t>
-  </si>
-  <si>
     <t>PANTC</t>
   </si>
   <si>
@@ -253,6 +192,72 @@
   </si>
   <si>
     <t>NA</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> energy</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> protein</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> carbohydrate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> fiber</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vitamin_c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  vitamin_a_IU</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vitamin_d</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vitamin_e</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> thiamin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> riboflavin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> niacin</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vitamin_b6</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> folate</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> vitamin_b12</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> calcium</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> phosphorus</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> magnesium</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> potassium</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> sodium</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> iron</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> zinc</t>
   </si>
 </sst>
 </file>
@@ -339,7 +344,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
@@ -381,10 +386,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
+    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1" applyProtection="1">
@@ -401,11 +403,10 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyProtection="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="165" fontId="7" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="top"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -416,6 +417,11 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -742,63 +748,63 @@
   <dimension ref="A1:CR51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6:X6"/>
+      <selection activeCell="A3" sqref="A3:A27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="12" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="13" x14ac:dyDescent="0.15"/>
   <cols>
-    <col min="1" max="1" width="23.85546875" style="2" customWidth="1"/>
-    <col min="2" max="2" width="14.85546875" style="2" customWidth="1"/>
-    <col min="3" max="33" width="10.7109375" style="2"/>
-    <col min="34" max="34" width="32.85546875" style="2" customWidth="1"/>
-    <col min="35" max="65" width="10.7109375" style="2"/>
-    <col min="66" max="66" width="37.7109375" style="2" customWidth="1"/>
-    <col min="67" max="16384" width="10.7109375" style="2"/>
+    <col min="1" max="1" width="23.83203125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="14.83203125" style="2" customWidth="1"/>
+    <col min="3" max="33" width="10.83203125" style="2"/>
+    <col min="34" max="34" width="32.83203125" style="2" customWidth="1"/>
+    <col min="35" max="65" width="10.83203125" style="2"/>
+    <col min="66" max="66" width="37.6640625" style="2" customWidth="1"/>
+    <col min="67" max="16384" width="10.83203125" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:96" s="3" customFormat="1" ht="13">
+    <row r="1" spans="1:96" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A1" s="1" t="s">
-        <v>66</v>
+        <v>44</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>67</v>
-      </c>
-      <c r="C1" s="21" t="s">
+        <v>45</v>
+      </c>
+      <c r="C1" s="20" t="s">
         <v>26</v>
       </c>
-      <c r="D1" s="21"/>
-      <c r="E1" s="22" t="s">
+      <c r="D1" s="20"/>
+      <c r="E1" s="21" t="s">
         <v>28</v>
       </c>
-      <c r="F1" s="23"/>
-      <c r="G1" s="22" t="s">
+      <c r="F1" s="22"/>
+      <c r="G1" s="21" t="s">
         <v>31</v>
       </c>
-      <c r="H1" s="23"/>
-      <c r="I1" s="23"/>
-      <c r="J1" s="23"/>
-      <c r="K1" s="23"/>
-      <c r="L1" s="23"/>
-      <c r="M1" s="19" t="s">
+      <c r="H1" s="22"/>
+      <c r="I1" s="22"/>
+      <c r="J1" s="22"/>
+      <c r="K1" s="22"/>
+      <c r="L1" s="22"/>
+      <c r="M1" s="18" t="s">
         <v>38</v>
       </c>
-      <c r="N1" s="20"/>
-      <c r="O1" s="20"/>
-      <c r="P1" s="20"/>
-      <c r="Q1" s="20"/>
-      <c r="R1" s="20"/>
-      <c r="S1" s="19" t="s">
+      <c r="N1" s="19"/>
+      <c r="O1" s="19"/>
+      <c r="P1" s="19"/>
+      <c r="Q1" s="19"/>
+      <c r="R1" s="19"/>
+      <c r="S1" s="18" t="s">
         <v>39</v>
       </c>
-      <c r="T1" s="20"/>
-      <c r="U1" s="20"/>
-      <c r="V1" s="19" t="s">
+      <c r="T1" s="19"/>
+      <c r="U1" s="19"/>
+      <c r="V1" s="18" t="s">
         <v>40</v>
       </c>
-      <c r="W1" s="20"/>
-      <c r="X1" s="20"/>
-    </row>
-    <row r="2" spans="1:96" s="3" customFormat="1">
+      <c r="W1" s="19"/>
+      <c r="X1" s="19"/>
+    </row>
+    <row r="2" spans="1:96" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="1" t="s">
@@ -898,8 +904,8 @@
       <c r="BK2" s="1"/>
       <c r="BL2" s="1"/>
       <c r="BM2" s="1"/>
-      <c r="BO2" s="18"/>
-      <c r="BP2" s="18"/>
+      <c r="BO2" s="24"/>
+      <c r="BP2" s="24"/>
       <c r="BQ2" s="15"/>
       <c r="BR2" s="15"/>
       <c r="BS2" s="15"/>
@@ -929,9 +935,9 @@
       <c r="CQ2" s="15"/>
       <c r="CR2" s="15"/>
     </row>
-    <row r="3" spans="1:96" ht="14">
-      <c r="A3" s="24" t="s">
-        <v>41</v>
+    <row r="3" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>47</v>
       </c>
       <c r="B3" s="4" t="s">
         <v>0</v>
@@ -1066,9 +1072,9 @@
       <c r="CQ3" s="5"/>
       <c r="CR3" s="5"/>
     </row>
-    <row r="4" spans="1:96" ht="14">
-      <c r="A4" s="24" t="s">
-        <v>42</v>
+    <row r="4" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>48</v>
       </c>
       <c r="B4" s="16" t="s">
         <v>4</v>
@@ -1203,9 +1209,9 @@
       <c r="CQ4" s="5"/>
       <c r="CR4" s="5"/>
     </row>
-    <row r="5" spans="1:96" ht="14">
-      <c r="A5" s="24" t="s">
-        <v>44</v>
+    <row r="5" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>50</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>5</v>
@@ -1303,8 +1309,8 @@
       <c r="BL5" s="8"/>
       <c r="BM5" s="8"/>
       <c r="BN5" s="3"/>
-      <c r="BO5" s="17"/>
-      <c r="BP5" s="17"/>
+      <c r="BO5" s="23"/>
+      <c r="BP5" s="23"/>
       <c r="BR5" s="5"/>
       <c r="BS5" s="5"/>
       <c r="BU5" s="5"/>
@@ -1328,9 +1334,9 @@
       <c r="CQ5" s="5"/>
       <c r="CR5" s="5"/>
     </row>
-    <row r="6" spans="1:96" ht="14">
-      <c r="A6" s="24" t="s">
-        <v>43</v>
+    <row r="6" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>49</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>6</v>
@@ -1342,64 +1348,64 @@
         <v>30</v>
       </c>
       <c r="E6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="F6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="G6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="H6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="J6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="K6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="L6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="M6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="N6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="O6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="P6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="Q6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="R6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="S6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="T6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="U6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="V6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="W6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="X6" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="AH6" s="3"/>
       <c r="AI6" s="4"/>
@@ -1453,18 +1459,18 @@
       <c r="CQ6" s="5"/>
       <c r="CR6" s="5"/>
     </row>
-    <row r="7" spans="1:96" ht="14">
-      <c r="A7" s="24" t="s">
-        <v>45</v>
+    <row r="7" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>51</v>
       </c>
       <c r="B7" s="14" t="s">
         <v>1</v>
       </c>
       <c r="C7" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="D7" s="13" t="s">
-        <v>68</v>
+        <v>46</v>
       </c>
       <c r="E7" s="12">
         <v>19</v>
@@ -1578,9 +1584,9 @@
       <c r="CQ7" s="5"/>
       <c r="CR7" s="5"/>
     </row>
-    <row r="8" spans="1:96" ht="14">
-      <c r="A8" s="24" t="s">
-        <v>55</v>
+    <row r="8" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>53</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>3</v>
@@ -1652,9 +1658,9 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="9" spans="1:96" ht="14">
-      <c r="A9" s="25" t="s">
-        <v>58</v>
+    <row r="9" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>52</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>2</v>
@@ -1726,9 +1732,9 @@
         <v>120</v>
       </c>
     </row>
-    <row r="10" spans="1:96" ht="14">
-      <c r="A10" s="24" t="s">
-        <v>56</v>
+    <row r="10" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A10" t="s">
+        <v>54</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>23</v>
@@ -1800,9 +1806,9 @@
         <v>5</v>
       </c>
     </row>
-    <row r="11" spans="1:96" ht="14">
-      <c r="A11" s="24" t="s">
-        <v>57</v>
+    <row r="11" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>55</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>17</v>
@@ -1874,9 +1880,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="12" spans="1:96" ht="14">
-      <c r="A12" s="24" t="s">
-        <v>59</v>
+    <row r="12" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A12" t="s">
+        <v>56</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>18</v>
@@ -1948,9 +1954,9 @@
         <v>1.4</v>
       </c>
     </row>
-    <row r="13" spans="1:96" ht="14">
-      <c r="A13" s="24" t="s">
-        <v>60</v>
+    <row r="13" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A13" t="s">
+        <v>57</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>19</v>
@@ -2022,9 +2028,9 @@
         <v>1.6</v>
       </c>
     </row>
-    <row r="14" spans="1:96" ht="14">
-      <c r="A14" s="24" t="s">
-        <v>61</v>
+    <row r="14" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A14" t="s">
+        <v>58</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>20</v>
@@ -2096,9 +2102,9 @@
         <v>17</v>
       </c>
     </row>
-    <row r="15" spans="1:96" ht="14">
-      <c r="A15" s="24" t="s">
-        <v>62</v>
+    <row r="15" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A15" t="s">
+        <v>59</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>21</v>
@@ -2170,9 +2176,9 @@
         <v>2</v>
       </c>
     </row>
-    <row r="16" spans="1:96" ht="14">
-      <c r="A16" s="24" t="s">
-        <v>63</v>
+    <row r="16" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A16" t="s">
+        <v>60</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>15</v>
@@ -2244,9 +2250,9 @@
         <v>500</v>
       </c>
     </row>
-    <row r="17" spans="1:96" ht="14">
-      <c r="A17" s="24" t="s">
-        <v>64</v>
+    <row r="17" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A17" t="s">
+        <v>61</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>24</v>
@@ -2318,9 +2324,9 @@
         <v>2.8</v>
       </c>
     </row>
-    <row r="18" spans="1:96" ht="14">
-      <c r="A18" s="24" t="s">
-        <v>65</v>
+    <row r="18" spans="1:96" ht="15" x14ac:dyDescent="0.2">
+      <c r="A18" s="17" t="s">
+        <v>43</v>
       </c>
       <c r="B18" s="14" t="s">
         <v>22</v>
@@ -2392,9 +2398,9 @@
         <v>7</v>
       </c>
     </row>
-    <row r="19" spans="1:96" ht="14">
-      <c r="A19" s="24" t="s">
-        <v>46</v>
+    <row r="19" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A19" t="s">
+        <v>62</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>7</v>
@@ -2466,9 +2472,9 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="20" spans="1:96" ht="14">
-      <c r="A20" s="24" t="s">
-        <v>47</v>
+    <row r="20" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A20" t="s">
+        <v>63</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>8</v>
@@ -2540,9 +2546,9 @@
         <v>700</v>
       </c>
     </row>
-    <row r="21" spans="1:96" ht="14">
-      <c r="A21" s="24" t="s">
-        <v>48</v>
+    <row r="21" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A21" t="s">
+        <v>64</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>9</v>
@@ -2614,9 +2620,9 @@
         <v>320</v>
       </c>
     </row>
-    <row r="22" spans="1:96" ht="14">
-      <c r="A22" s="24" t="s">
-        <v>49</v>
+    <row r="22" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A22" t="s">
+        <v>65</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>10</v>
@@ -2688,9 +2694,9 @@
         <v>5.0999999999999996</v>
       </c>
     </row>
-    <row r="23" spans="1:96" ht="14">
-      <c r="A23" s="24" t="s">
-        <v>50</v>
+    <row r="23" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A23" t="s">
+        <v>66</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>11</v>
@@ -2762,9 +2768,9 @@
         <v>1.5</v>
       </c>
     </row>
-    <row r="24" spans="1:96" ht="14">
-      <c r="A24" s="24" t="s">
-        <v>51</v>
+    <row r="24" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A24" t="s">
+        <v>67</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>12</v>
@@ -2836,9 +2842,9 @@
         <v>9</v>
       </c>
     </row>
-    <row r="25" spans="1:96" ht="14">
-      <c r="A25" s="24" t="s">
-        <v>52</v>
+    <row r="25" spans="1:96" x14ac:dyDescent="0.15">
+      <c r="A25" t="s">
+        <v>68</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>13</v>
@@ -2910,9 +2916,9 @@
         <v>12</v>
       </c>
     </row>
-    <row r="26" spans="1:96" ht="14">
-      <c r="A26" s="24" t="s">
-        <v>53</v>
+    <row r="26" spans="1:96" ht="15" x14ac:dyDescent="0.2">
+      <c r="A26" s="17" t="s">
+        <v>41</v>
       </c>
       <c r="B26" s="16" t="s">
         <v>16</v>
@@ -2984,9 +2990,9 @@
         <v>1300</v>
       </c>
     </row>
-    <row r="27" spans="1:96" ht="14">
-      <c r="A27" s="24" t="s">
-        <v>54</v>
+    <row r="27" spans="1:96" ht="15" x14ac:dyDescent="0.2">
+      <c r="A27" s="17" t="s">
+        <v>42</v>
       </c>
       <c r="B27" s="14" t="s">
         <v>14</v>
@@ -3058,7 +3064,7 @@
         <v>2.6</v>
       </c>
     </row>
-    <row r="28" spans="1:96">
+    <row r="28" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A28" s="4"/>
       <c r="B28" s="4"/>
       <c r="C28" s="6"/>
@@ -3133,7 +3139,7 @@
       <c r="CQ28" s="8"/>
       <c r="CR28" s="8"/>
     </row>
-    <row r="29" spans="1:96">
+    <row r="29" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A29" s="4"/>
       <c r="B29" s="4"/>
       <c r="C29" s="4"/>
@@ -3183,8 +3189,8 @@
       <c r="BK29" s="11"/>
       <c r="BL29" s="11"/>
       <c r="BM29" s="11"/>
-      <c r="BO29" s="17"/>
-      <c r="BP29" s="17"/>
+      <c r="BO29" s="23"/>
+      <c r="BP29" s="23"/>
       <c r="BR29" s="5"/>
       <c r="BS29" s="5"/>
       <c r="BU29" s="8"/>
@@ -3208,7 +3214,7 @@
       <c r="CQ29" s="8"/>
       <c r="CR29" s="8"/>
     </row>
-    <row r="30" spans="1:96">
+    <row r="30" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A30" s="4"/>
       <c r="B30" s="4"/>
       <c r="C30" s="4"/>
@@ -3258,8 +3264,8 @@
       <c r="BK30" s="8"/>
       <c r="BL30" s="8"/>
       <c r="BM30" s="8"/>
-      <c r="BO30" s="17"/>
-      <c r="BP30" s="17"/>
+      <c r="BO30" s="23"/>
+      <c r="BP30" s="23"/>
       <c r="BR30" s="5"/>
       <c r="BS30" s="5"/>
       <c r="BU30" s="5"/>
@@ -3283,7 +3289,7 @@
       <c r="CQ30" s="5"/>
       <c r="CR30" s="5"/>
     </row>
-    <row r="31" spans="1:96">
+    <row r="31" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A31" s="4"/>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -3333,8 +3339,8 @@
       <c r="BK31" s="11"/>
       <c r="BL31" s="11"/>
       <c r="BM31" s="11"/>
-      <c r="BO31" s="17"/>
-      <c r="BP31" s="17"/>
+      <c r="BO31" s="23"/>
+      <c r="BP31" s="23"/>
       <c r="BR31" s="5"/>
       <c r="BS31" s="5"/>
       <c r="BU31" s="8"/>
@@ -3358,7 +3364,7 @@
       <c r="CQ31" s="8"/>
       <c r="CR31" s="8"/>
     </row>
-    <row r="32" spans="1:96">
+    <row r="32" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A32" s="4"/>
       <c r="B32" s="4"/>
       <c r="C32" s="4"/>
@@ -3408,8 +3414,8 @@
       <c r="BK32" s="8"/>
       <c r="BL32" s="8"/>
       <c r="BM32" s="8"/>
-      <c r="BO32" s="17"/>
-      <c r="BP32" s="17"/>
+      <c r="BO32" s="23"/>
+      <c r="BP32" s="23"/>
       <c r="BR32" s="5"/>
       <c r="BS32" s="5"/>
       <c r="BU32" s="8"/>
@@ -3433,7 +3439,7 @@
       <c r="CQ32" s="8"/>
       <c r="CR32" s="8"/>
     </row>
-    <row r="33" spans="1:96">
+    <row r="33" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A33" s="4"/>
       <c r="B33" s="4"/>
       <c r="C33" s="4"/>
@@ -3483,8 +3489,8 @@
       <c r="BK33" s="11"/>
       <c r="BL33" s="11"/>
       <c r="BM33" s="11"/>
-      <c r="BO33" s="17"/>
-      <c r="BP33" s="17"/>
+      <c r="BO33" s="23"/>
+      <c r="BP33" s="23"/>
       <c r="BR33" s="5"/>
       <c r="BS33" s="5"/>
       <c r="BU33" s="8"/>
@@ -3508,7 +3514,7 @@
       <c r="CQ33" s="8"/>
       <c r="CR33" s="8"/>
     </row>
-    <row r="34" spans="1:96">
+    <row r="34" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A34" s="4"/>
       <c r="B34" s="4"/>
       <c r="C34" s="4"/>
@@ -3583,7 +3589,7 @@
       <c r="CQ34" s="8"/>
       <c r="CR34" s="8"/>
     </row>
-    <row r="35" spans="1:96">
+    <row r="35" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A35" s="4"/>
       <c r="B35" s="4"/>
       <c r="C35" s="4"/>
@@ -3633,8 +3639,8 @@
       <c r="BK35" s="4"/>
       <c r="BL35" s="4"/>
       <c r="BM35" s="4"/>
-      <c r="BO35" s="17"/>
-      <c r="BP35" s="17"/>
+      <c r="BO35" s="23"/>
+      <c r="BP35" s="23"/>
       <c r="BR35" s="5"/>
       <c r="BS35" s="5"/>
       <c r="BU35" s="5"/>
@@ -3658,7 +3664,7 @@
       <c r="CQ35" s="5"/>
       <c r="CR35" s="5"/>
     </row>
-    <row r="36" spans="1:96">
+    <row r="36" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A36" s="4"/>
       <c r="B36" s="4"/>
       <c r="E36" s="6"/>
@@ -3731,7 +3737,7 @@
       <c r="CQ36" s="5"/>
       <c r="CR36" s="5"/>
     </row>
-    <row r="37" spans="1:96">
+    <row r="37" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A37" s="4"/>
       <c r="B37" s="4"/>
       <c r="E37" s="6"/>
@@ -3779,7 +3785,7 @@
       <c r="CQ37" s="5"/>
       <c r="CR37" s="5"/>
     </row>
-    <row r="38" spans="1:96">
+    <row r="38" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A38" s="4"/>
       <c r="B38" s="4"/>
       <c r="E38" s="10"/>
@@ -3803,7 +3809,7 @@
       <c r="W38" s="10"/>
       <c r="X38" s="10"/>
     </row>
-    <row r="39" spans="1:96">
+    <row r="39" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A39" s="4"/>
       <c r="B39" s="4"/>
       <c r="E39" s="6"/>
@@ -3827,7 +3833,7 @@
       <c r="W39" s="6"/>
       <c r="X39" s="6"/>
     </row>
-    <row r="40" spans="1:96">
+    <row r="40" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A40" s="4"/>
       <c r="B40" s="4"/>
       <c r="E40" s="6"/>
@@ -3851,7 +3857,7 @@
       <c r="W40" s="6"/>
       <c r="X40" s="6"/>
     </row>
-    <row r="41" spans="1:96">
+    <row r="41" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A41" s="4"/>
       <c r="B41" s="4"/>
       <c r="E41" s="6"/>
@@ -3875,7 +3881,7 @@
       <c r="W41" s="6"/>
       <c r="X41" s="6"/>
     </row>
-    <row r="42" spans="1:96">
+    <row r="42" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A42" s="4"/>
       <c r="B42" s="4"/>
       <c r="E42" s="6"/>
@@ -3899,7 +3905,7 @@
       <c r="W42" s="6"/>
       <c r="X42" s="6"/>
     </row>
-    <row r="43" spans="1:96">
+    <row r="43" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A43" s="4"/>
       <c r="B43" s="4"/>
       <c r="E43" s="10"/>
@@ -3923,38 +3929,32 @@
       <c r="W43" s="10"/>
       <c r="X43" s="10"/>
     </row>
-    <row r="44" spans="1:96" ht="13">
+    <row r="44" spans="1:96" x14ac:dyDescent="0.15">
       <c r="B44"/>
     </row>
-    <row r="45" spans="1:96" ht="13">
+    <row r="45" spans="1:96" x14ac:dyDescent="0.15">
       <c r="B45"/>
     </row>
-    <row r="46" spans="1:96" ht="13">
+    <row r="46" spans="1:96" x14ac:dyDescent="0.15">
       <c r="B46"/>
     </row>
-    <row r="47" spans="1:96" ht="13">
+    <row r="47" spans="1:96" x14ac:dyDescent="0.15">
       <c r="B47"/>
     </row>
-    <row r="48" spans="1:96" ht="13">
+    <row r="48" spans="1:96" x14ac:dyDescent="0.15">
       <c r="B48"/>
     </row>
-    <row r="49" spans="2:2" ht="13">
+    <row r="49" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B49"/>
     </row>
-    <row r="50" spans="2:2" ht="13">
+    <row r="50" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B50"/>
     </row>
-    <row r="51" spans="2:2" ht="13">
+    <row r="51" spans="2:2" x14ac:dyDescent="0.15">
       <c r="B51"/>
     </row>
   </sheetData>
   <mergeCells count="14">
-    <mergeCell ref="V1:X1"/>
-    <mergeCell ref="C1:D1"/>
-    <mergeCell ref="E1:F1"/>
-    <mergeCell ref="G1:L1"/>
-    <mergeCell ref="M1:R1"/>
-    <mergeCell ref="S1:U1"/>
     <mergeCell ref="BO31:BP31"/>
     <mergeCell ref="BO32:BP32"/>
     <mergeCell ref="BO33:BP33"/>
@@ -3963,14 +3963,15 @@
     <mergeCell ref="BO5:BP5"/>
     <mergeCell ref="BO29:BP29"/>
     <mergeCell ref="BO30:BP30"/>
+    <mergeCell ref="V1:X1"/>
+    <mergeCell ref="C1:D1"/>
+    <mergeCell ref="E1:F1"/>
+    <mergeCell ref="G1:L1"/>
+    <mergeCell ref="M1:R1"/>
+    <mergeCell ref="S1:U1"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Substantively minor changes. - moved old code from nutrientModeling to another script - a few cleanups in the other scripts - added the new nutrient lookup spreadsheet (V6)
</commit_message>
<xml_diff>
--- a/data/DRI EAR valuesV2.xlsx
+++ b/data/DRI EAR valuesV2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26207"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26311"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="1040" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="2480" yWindow="820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DRI -RDA&amp;AI" sheetId="2" r:id="rId1"/>
@@ -194,70 +194,70 @@
     <t>NA</t>
   </si>
   <si>
-    <t xml:space="preserve"> energy</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> protein</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fat</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> carbohydrate</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> fiber</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vitamin_c</t>
-  </si>
-  <si>
-    <t xml:space="preserve">  vitamin_a_IU</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vitamin_d</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vitamin_e</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> thiamin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> riboflavin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> niacin</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vitamin_b6</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> folate</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> vitamin_b12</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> calcium</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> phosphorus</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> magnesium</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> potassium</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> sodium</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> iron</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> zinc</t>
+    <t>energy</t>
+  </si>
+  <si>
+    <t>protein</t>
+  </si>
+  <si>
+    <t>carbohydrate</t>
+  </si>
+  <si>
+    <t>fat</t>
+  </si>
+  <si>
+    <t>fiber</t>
+  </si>
+  <si>
+    <t>vitamin_a_IU</t>
+  </si>
+  <si>
+    <t>vitamin_c</t>
+  </si>
+  <si>
+    <t>vitamin_d</t>
+  </si>
+  <si>
+    <t>vitamin_e</t>
+  </si>
+  <si>
+    <t>thiamin</t>
+  </si>
+  <si>
+    <t>riboflavin</t>
+  </si>
+  <si>
+    <t>niacin</t>
+  </si>
+  <si>
+    <t>vitamin_b6</t>
+  </si>
+  <si>
+    <t>folate</t>
+  </si>
+  <si>
+    <t>vitamin_b12</t>
+  </si>
+  <si>
+    <t>calcium</t>
+  </si>
+  <si>
+    <t>phosphorus</t>
+  </si>
+  <si>
+    <t>magnesium</t>
+  </si>
+  <si>
+    <t>potassium</t>
+  </si>
+  <si>
+    <t>sodium</t>
+  </si>
+  <si>
+    <t>iron</t>
+  </si>
+  <si>
+    <t>zinc</t>
   </si>
 </sst>
 </file>
@@ -1211,7 +1211,7 @@
     </row>
     <row r="5" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B5" s="16" t="s">
         <v>5</v>
@@ -1336,7 +1336,7 @@
     </row>
     <row r="6" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>50</v>
       </c>
       <c r="B6" s="16" t="s">
         <v>6</v>
@@ -1586,7 +1586,7 @@
     </row>
     <row r="8" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>3</v>
@@ -1660,7 +1660,7 @@
     </row>
     <row r="9" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>2</v>

</xml_diff>

<commit_message>
Too many changes to document.
</commit_message>
<xml_diff>
--- a/data/DRI EAR valuesV2.xlsx
+++ b/data/DRI EAR valuesV2.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26311"/>
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="26408"/>
   <workbookPr date1904="1" showInkAnnotation="0" autoCompressPictures="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -9,12 +9,12 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2480" yWindow="820" windowWidth="25600" windowHeight="16060" tabRatio="500"/>
+    <workbookView xWindow="-20740" yWindow="-3820" windowWidth="18040" windowHeight="16060" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="DRI -RDA&amp;AI" sheetId="2" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="130407" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="69">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="71">
   <si>
     <t>Energy (kcal/d)</t>
     <phoneticPr fontId="2" type="noConversion"/>
@@ -209,9 +209,6 @@
     <t>fiber</t>
   </si>
   <si>
-    <t>vitamin_a_IU</t>
-  </si>
-  <si>
     <t>vitamin_c</t>
   </si>
   <si>
@@ -258,6 +255,15 @@
   </si>
   <si>
     <t>zinc</t>
+  </si>
+  <si>
+    <t>min</t>
+  </si>
+  <si>
+    <t>max</t>
+  </si>
+  <si>
+    <t>vitamin_a</t>
   </si>
 </sst>
 </file>
@@ -339,8 +345,10 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
@@ -410,9 +418,11 @@
       <protection locked="0"/>
     </xf>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="5">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -755,7 +765,8 @@
   <cols>
     <col min="1" max="1" width="23.83203125" style="2" customWidth="1"/>
     <col min="2" max="2" width="14.83203125" style="2" customWidth="1"/>
-    <col min="3" max="33" width="10.83203125" style="2"/>
+    <col min="3" max="24" width="10.83203125" style="2" customWidth="1"/>
+    <col min="25" max="33" width="10.83203125" style="2"/>
     <col min="34" max="34" width="32.83203125" style="2" customWidth="1"/>
     <col min="35" max="65" width="10.83203125" style="2"/>
     <col min="66" max="66" width="37.6640625" style="2" customWidth="1"/>
@@ -803,6 +814,12 @@
       </c>
       <c r="W1" s="19"/>
       <c r="X1" s="19"/>
+      <c r="Y1" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z1" s="3" t="s">
+        <v>69</v>
+      </c>
     </row>
     <row r="2" spans="1:96" s="3" customFormat="1" x14ac:dyDescent="0.15">
       <c r="A2" s="1"/>
@@ -1007,6 +1024,14 @@
       </c>
       <c r="X3" s="12">
         <v>2750</v>
+      </c>
+      <c r="Y3" s="13">
+        <f>MIN(C3:X3)</f>
+        <v>570</v>
+      </c>
+      <c r="Z3" s="13">
+        <f>MAX(C3:X3)</f>
+        <v>2755</v>
       </c>
       <c r="AH3" s="3"/>
       <c r="AI3" s="4"/>
@@ -1145,6 +1170,14 @@
       <c r="X4" s="12">
         <v>71</v>
       </c>
+      <c r="Y4" s="13">
+        <f t="shared" ref="Y4:Y27" si="0">MIN(C4:X4)</f>
+        <v>9.1</v>
+      </c>
+      <c r="Z4" s="13">
+        <f t="shared" ref="Z4:Z27" si="1">MAX(C4:X4)</f>
+        <v>71</v>
+      </c>
       <c r="AH4" s="3"/>
       <c r="AI4" s="4"/>
       <c r="AJ4" s="4"/>
@@ -1282,6 +1315,14 @@
       <c r="X5" s="12">
         <v>210</v>
       </c>
+      <c r="Y5" s="13">
+        <f t="shared" si="0"/>
+        <v>60</v>
+      </c>
+      <c r="Z5" s="13">
+        <f t="shared" si="1"/>
+        <v>210</v>
+      </c>
       <c r="AH5" s="3"/>
       <c r="AI5" s="4"/>
       <c r="AJ5" s="4"/>
@@ -1407,6 +1448,14 @@
       <c r="X6" s="13" t="s">
         <v>46</v>
       </c>
+      <c r="Y6" s="13">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="Z6" s="13">
+        <f t="shared" si="1"/>
+        <v>31</v>
+      </c>
       <c r="AH6" s="3"/>
       <c r="AI6" s="4"/>
       <c r="AJ6" s="4"/>
@@ -1532,6 +1581,14 @@
       <c r="X7" s="12">
         <v>29</v>
       </c>
+      <c r="Y7" s="13">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="Z7" s="13">
+        <f t="shared" si="1"/>
+        <v>38</v>
+      </c>
       <c r="AH7" s="3"/>
       <c r="AI7" s="4"/>
       <c r="AJ7" s="4"/>
@@ -1586,7 +1643,7 @@
     </row>
     <row r="8" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>52</v>
+        <v>70</v>
       </c>
       <c r="B8" s="14" t="s">
         <v>3</v>
@@ -1657,10 +1714,18 @@
       <c r="X8" s="6">
         <v>1300</v>
       </c>
+      <c r="Y8" s="13">
+        <f t="shared" si="0"/>
+        <v>300</v>
+      </c>
+      <c r="Z8" s="13">
+        <f t="shared" si="1"/>
+        <v>1300</v>
+      </c>
     </row>
     <row r="9" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A9" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B9" s="14" t="s">
         <v>2</v>
@@ -1731,10 +1796,18 @@
       <c r="X9" s="6">
         <v>120</v>
       </c>
+      <c r="Y9" s="13">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="Z9" s="13">
+        <f t="shared" si="1"/>
+        <v>120</v>
+      </c>
     </row>
     <row r="10" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B10" s="14" t="s">
         <v>23</v>
@@ -1805,10 +1878,18 @@
       <c r="X10" s="6">
         <v>5</v>
       </c>
+      <c r="Y10" s="13">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="Z10" s="13">
+        <f t="shared" si="1"/>
+        <v>15</v>
+      </c>
     </row>
     <row r="11" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A11" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>17</v>
@@ -1879,10 +1960,18 @@
       <c r="X11" s="6">
         <v>19</v>
       </c>
+      <c r="Y11" s="13">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="Z11" s="13">
+        <f t="shared" si="1"/>
+        <v>19</v>
+      </c>
     </row>
     <row r="12" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A12" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B12" s="14" t="s">
         <v>18</v>
@@ -1953,10 +2042,18 @@
       <c r="X12" s="10">
         <v>1.4</v>
       </c>
+      <c r="Y12" s="13">
+        <f t="shared" si="0"/>
+        <v>0.2</v>
+      </c>
+      <c r="Z12" s="13">
+        <f t="shared" si="1"/>
+        <v>1.9</v>
+      </c>
     </row>
     <row r="13" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A13" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B13" s="14" t="s">
         <v>19</v>
@@ -2027,10 +2124,18 @@
       <c r="X13" s="10">
         <v>1.6</v>
       </c>
+      <c r="Y13" s="13">
+        <f t="shared" si="0"/>
+        <v>0.3</v>
+      </c>
+      <c r="Z13" s="13">
+        <f t="shared" si="1"/>
+        <v>1.6</v>
+      </c>
     </row>
     <row r="14" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A14" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B14" s="14" t="s">
         <v>20</v>
@@ -2101,10 +2206,18 @@
       <c r="X14" s="6">
         <v>17</v>
       </c>
+      <c r="Y14" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Z14" s="13">
+        <f t="shared" si="1"/>
+        <v>18</v>
+      </c>
     </row>
     <row r="15" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A15" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B15" s="14" t="s">
         <v>21</v>
@@ -2175,10 +2288,18 @@
       <c r="X15" s="10">
         <v>2</v>
       </c>
+      <c r="Y15" s="13">
+        <f t="shared" si="0"/>
+        <v>0.1</v>
+      </c>
+      <c r="Z15" s="13">
+        <f t="shared" si="1"/>
+        <v>2</v>
+      </c>
     </row>
     <row r="16" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A16" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B16" s="14" t="s">
         <v>15</v>
@@ -2249,10 +2370,18 @@
       <c r="X16" s="6">
         <v>500</v>
       </c>
+      <c r="Y16" s="13">
+        <f t="shared" si="0"/>
+        <v>65</v>
+      </c>
+      <c r="Z16" s="13">
+        <f t="shared" si="1"/>
+        <v>600</v>
+      </c>
     </row>
     <row r="17" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B17" s="14" t="s">
         <v>24</v>
@@ -2321,6 +2450,14 @@
         <v>2.8</v>
       </c>
       <c r="X17" s="10">
+        <v>2.8</v>
+      </c>
+      <c r="Y17" s="13">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="Z17" s="13">
+        <f t="shared" si="1"/>
         <v>2.8</v>
       </c>
     </row>
@@ -2397,10 +2534,18 @@
       <c r="X18" s="2">
         <v>7</v>
       </c>
+      <c r="Y18" s="13">
+        <f t="shared" si="0"/>
+        <v>1.7</v>
+      </c>
+      <c r="Z18" s="13">
+        <f t="shared" si="1"/>
+        <v>7</v>
+      </c>
     </row>
     <row r="19" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" s="16" t="s">
         <v>7</v>
@@ -2471,10 +2616,18 @@
       <c r="X19" s="6">
         <v>1000</v>
       </c>
+      <c r="Y19" s="13">
+        <f t="shared" si="0"/>
+        <v>210</v>
+      </c>
+      <c r="Z19" s="13">
+        <f t="shared" si="1"/>
+        <v>1300</v>
+      </c>
     </row>
     <row r="20" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A20" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B20" s="16" t="s">
         <v>8</v>
@@ -2545,10 +2698,18 @@
       <c r="X20" s="6">
         <v>700</v>
       </c>
+      <c r="Y20" s="13">
+        <f t="shared" si="0"/>
+        <v>100</v>
+      </c>
+      <c r="Z20" s="13">
+        <f t="shared" si="1"/>
+        <v>1250</v>
+      </c>
     </row>
     <row r="21" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A21" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B21" s="16" t="s">
         <v>9</v>
@@ -2619,10 +2780,18 @@
       <c r="X21" s="6">
         <v>320</v>
       </c>
+      <c r="Y21" s="13">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="Z21" s="13">
+        <f t="shared" si="1"/>
+        <v>420</v>
+      </c>
     </row>
     <row r="22" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A22" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B22" s="14" t="s">
         <v>10</v>
@@ -2693,10 +2862,18 @@
       <c r="X22" s="2">
         <v>5.0999999999999996</v>
       </c>
+      <c r="Y22" s="13">
+        <f t="shared" si="0"/>
+        <v>0.4</v>
+      </c>
+      <c r="Z22" s="13">
+        <f t="shared" si="1"/>
+        <v>5.0999999999999996</v>
+      </c>
     </row>
     <row r="23" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A23" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B23" s="14" t="s">
         <v>11</v>
@@ -2767,10 +2944,18 @@
       <c r="X23" s="2">
         <v>1.5</v>
       </c>
+      <c r="Y23" s="13">
+        <f t="shared" si="0"/>
+        <v>0.12</v>
+      </c>
+      <c r="Z23" s="13">
+        <f t="shared" si="1"/>
+        <v>1.5</v>
+      </c>
     </row>
     <row r="24" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A24" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B24" s="16" t="s">
         <v>12</v>
@@ -2841,10 +3026,18 @@
       <c r="X24" s="10">
         <v>9</v>
       </c>
+      <c r="Y24" s="13">
+        <f t="shared" si="0"/>
+        <v>0.27</v>
+      </c>
+      <c r="Z24" s="13">
+        <f t="shared" si="1"/>
+        <v>27</v>
+      </c>
     </row>
     <row r="25" spans="1:96" x14ac:dyDescent="0.15">
       <c r="A25" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B25" s="14" t="s">
         <v>13</v>
@@ -2914,6 +3107,14 @@
       </c>
       <c r="X25" s="10">
         <v>12</v>
+      </c>
+      <c r="Y25" s="13">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="Z25" s="13">
+        <f t="shared" si="1"/>
+        <v>13</v>
       </c>
     </row>
     <row r="26" spans="1:96" ht="15" x14ac:dyDescent="0.2">
@@ -2989,6 +3190,14 @@
       <c r="X26" s="7">
         <v>1300</v>
       </c>
+      <c r="Y26" s="13">
+        <f t="shared" si="0"/>
+        <v>200</v>
+      </c>
+      <c r="Z26" s="13">
+        <f t="shared" si="1"/>
+        <v>1300</v>
+      </c>
     </row>
     <row r="27" spans="1:96" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="17" t="s">
@@ -3061,6 +3270,14 @@
         <v>2.6</v>
       </c>
       <c r="X27" s="2">
+        <v>2.6</v>
+      </c>
+      <c r="Y27" s="13">
+        <f t="shared" si="0"/>
+        <v>3.0000000000000001E-3</v>
+      </c>
+      <c r="Z27" s="13">
+        <f t="shared" si="1"/>
         <v>2.6</v>
       </c>
     </row>

</xml_diff>